<commit_message>
010817 psp presentation update
</commit_message>
<xml_diff>
--- a/projects/psp/refined_data/google_disc_year.xlsx
+++ b/projects/psp/refined_data/google_disc_year.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
@@ -212,13 +212,20 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2800" baseline="0"/>
-              <a:t> PPP Through Google Search</a:t>
+              <a:t> PSP Through Google Search</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="2800"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.249524355078303"/>
+          <c:y val="0.0205761316872428"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -234,7 +241,9 @@
             <c:v>2010</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="3175"/>
+            <a:ln w="19050">
+              <a:prstDash val="sysDash"/>
+            </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -337,7 +346,7 @@
             <c:v>2011</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="3175">
+            <a:ln w="19050">
               <a:prstDash val="sysDash"/>
             </a:ln>
           </c:spPr>
@@ -442,7 +451,7 @@
             <c:v>2012</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="3175">
+            <a:ln w="19050">
               <a:prstDash val="sysDash"/>
             </a:ln>
           </c:spPr>
@@ -547,7 +556,7 @@
             <c:v>2013</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="3175">
+            <a:ln w="19050">
               <a:prstDash val="sysDash"/>
             </a:ln>
           </c:spPr>
@@ -652,7 +661,7 @@
             <c:v>2014</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="3175">
+            <a:ln w="19050">
               <a:prstDash val="sysDash"/>
             </a:ln>
           </c:spPr>
@@ -757,7 +766,7 @@
             <c:v>2015</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="3175">
+            <a:ln w="19050">
               <a:prstDash val="sysDash"/>
             </a:ln>
           </c:spPr>
@@ -1069,11 +1078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134529240"/>
-        <c:axId val="2103169592"/>
+        <c:axId val="2113456680"/>
+        <c:axId val="2113454632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2134529240"/>
+        <c:axId val="2113456680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103169592"/>
+        <c:crossAx val="2113454632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1100,7 +1109,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103169592"/>
+        <c:axId val="2113454632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1121,7 +1130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134529240"/>
+        <c:crossAx val="2113456680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2638,11 +2647,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2087539992"/>
-        <c:axId val="2087383208"/>
+        <c:axId val="2144263752"/>
+        <c:axId val="2144265160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2087539992"/>
+        <c:axId val="2144263752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2651,7 +2660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087383208"/>
+        <c:crossAx val="2144265160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2659,7 +2668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087383208"/>
+        <c:axId val="2144265160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2670,14 +2679,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087539992"/>
+        <c:crossAx val="2144263752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3087,7 +3095,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:M9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>